<commit_message>
GICS Sektoren Durchschnitte funktionieren
</commit_message>
<xml_diff>
--- a/excel_data/output.xlsx
+++ b/excel_data/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -168,7 +168,7 @@
     <t>Focus-Durchschnitt</t>
   </si>
   <si>
-    <t>Sektor-Durchschnitt</t>
+    <t>GICS-Sektor-Durchschnitt</t>
   </si>
   <si>
     <t>Zeile 1</t>
@@ -183,10 +183,7 @@
     <t>Focus-Ø (11 Unternehmen)</t>
   </si>
   <si>
-    <t>Sektor-Ø (4 Unternehmen)</t>
-  </si>
-  <si>
-    <t>Sektor-Ø (11 Unternehmen)</t>
+    <t>GICS-Sektor-Ø (Refinitiv-Branchendurchschnitt)</t>
   </si>
   <si>
     <t>826,300,000</t>
@@ -733,13 +730,13 @@
         <v>38.1345</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -765,13 +762,13 @@
         <v>-13.7552</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -797,13 +794,13 @@
         <v>-23.5126</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -829,13 +826,13 @@
         <v>-10.3557</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -861,13 +858,13 @@
         <v>-2.4463</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -893,13 +890,13 @@
         <v>3.0822</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -925,13 +922,13 @@
         <v>10.3658</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -957,13 +954,13 @@
         <v>7.1215</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -989,13 +986,13 @@
         <v>3.3866</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1021,13 +1018,13 @@
         <v>22.8146</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1053,13 +1050,13 @@
         <v>24.0117</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1085,13 +1082,13 @@
         <v>-3.5507</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1114,13 +1111,13 @@
         <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1143,13 +1140,13 @@
         <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1175,16 +1172,16 @@
         <v>-4.898</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1195,7 +1192,7 @@
         <v>-4.415934615384616</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1206,7 +1203,7 @@
         <v>6.654155555555556</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1223,7 +1220,7 @@
         <v>-2.37225</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1240,7 +1237,7 @@
         <v>6.654155555555556</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1250,8 +1247,17 @@
       <c r="F21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>1086058007.1146</v>
+      </c>
+      <c r="I21">
+        <v>925133996.1862</v>
+      </c>
+      <c r="J21">
+        <v>1165965874.6132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1259,7 +1265,16 @@
         <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="H22">
+        <v>3056797240.6806</v>
+      </c>
+      <c r="I22">
+        <v>2926006346.5578</v>
+      </c>
+      <c r="J22">
+        <v>3528485841.2753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no more double search for average, everything saved in cache
</commit_message>
<xml_diff>
--- a/excel_data/output.xlsx
+++ b/excel_data/output.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <name val="Calibri"/>
@@ -142,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -169,6 +171,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -184,10 +189,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -575,7 +580,7 @@
     <col width="26" customWidth="1" min="6" max="6"/>
     <col width="30" customWidth="1" min="7" max="7"/>
     <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="17" customWidth="1" min="9" max="9"/>
     <col width="18" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
@@ -685,7 +690,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H3" s="7" t="inlineStr"/>
+      <c r="H3" s="10" t="n">
+        <v>7.4109</v>
+      </c>
       <c r="I3" s="7" t="inlineStr">
         <is>
           <t>6,233,000,000</t>
@@ -698,48 +705,50 @@
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr">
         <is>
           <t>Kering SA</t>
         </is>
       </c>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="B4" s="12" t="inlineStr">
         <is>
           <t>PRTP.PA</t>
         </is>
       </c>
-      <c r="C4" s="12" t="inlineStr">
+      <c r="C4" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D4" s="13" t="inlineStr">
+      <c r="D4" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E4" s="13" t="inlineStr">
+      <c r="E4" s="14" t="inlineStr">
         <is>
           <t>High Luxury Segment</t>
         </is>
       </c>
-      <c r="F4" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G4" s="14" t="inlineStr">
+      <c r="F4" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G4" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H4" s="12" t="inlineStr"/>
-      <c r="I4" s="12" t="inlineStr">
+      <c r="H4" s="16" t="n">
+        <v>-41.253</v>
+      </c>
+      <c r="I4" s="13" t="inlineStr">
         <is>
           <t>2,489,000,000</t>
         </is>
       </c>
-      <c r="J4" s="12" t="inlineStr">
+      <c r="J4" s="13" t="inlineStr">
         <is>
           <t>5,493,000,000</t>
         </is>
@@ -781,7 +790,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H5" s="7" t="inlineStr"/>
+      <c r="H5" s="10" t="n">
+        <v>23.5162</v>
+      </c>
       <c r="I5" s="7" t="inlineStr">
         <is>
           <t>1,295,743,000</t>
@@ -794,48 +805,50 @@
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>Burberry Group PLC</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>BRBY.L</t>
         </is>
       </c>
-      <c r="C6" s="12" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D6" s="13" t="inlineStr">
+      <c r="D6" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>High Luxury Segment</t>
         </is>
       </c>
-      <c r="F6" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G6" s="14" t="inlineStr">
+      <c r="F6" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G6" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H6" s="12" t="inlineStr"/>
-      <c r="I6" s="12" t="inlineStr">
+      <c r="H6" s="16" t="n">
+        <v>-50.3389</v>
+      </c>
+      <c r="I6" s="13" t="inlineStr">
         <is>
           <t>57,000,000</t>
         </is>
       </c>
-      <c r="J6" s="12" t="inlineStr">
+      <c r="J6" s="13" t="inlineStr">
         <is>
           <t>639,000,000</t>
         </is>
@@ -877,7 +890,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H7" s="7" t="inlineStr"/>
+      <c r="H7" s="10" t="n">
+        <v>-46.601</v>
+      </c>
       <c r="I7" s="7" t="inlineStr">
         <is>
           <t>38,204,000</t>
@@ -890,48 +905,50 @@
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr">
         <is>
           <t>Brunello Cucinelli SpA</t>
         </is>
       </c>
-      <c r="B8" s="11" t="inlineStr">
+      <c r="B8" s="12" t="inlineStr">
         <is>
           <t>BCU.MI</t>
         </is>
       </c>
-      <c r="C8" s="12" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D8" s="13" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E8" s="13" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>High Luxury Segment</t>
         </is>
       </c>
-      <c r="F8" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G8" s="14" t="inlineStr">
+      <c r="F8" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G8" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H8" s="12" t="inlineStr"/>
-      <c r="I8" s="12" t="inlineStr">
+      <c r="H8" s="16" t="n">
+        <v>4.7968</v>
+      </c>
+      <c r="I8" s="13" t="inlineStr">
         <is>
           <t>211,541,000</t>
         </is>
       </c>
-      <c r="J8" s="12" t="inlineStr">
+      <c r="J8" s="13" t="inlineStr">
         <is>
           <t>134,498,000</t>
         </is>
@@ -973,7 +990,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H9" s="7" t="inlineStr"/>
+      <c r="H9" s="10" t="n">
+        <v>-30.8556</v>
+      </c>
       <c r="I9" s="7" t="inlineStr">
         <is>
           <t>184,020,000</t>
@@ -986,48 +1005,50 @@
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
-      <c r="A10" s="10" t="inlineStr">
+      <c r="A10" s="11" t="inlineStr">
         <is>
           <t>Ralph Lauren Corp</t>
         </is>
       </c>
-      <c r="B10" s="11" t="inlineStr">
+      <c r="B10" s="12" t="inlineStr">
         <is>
           <t>RL.N</t>
         </is>
       </c>
-      <c r="C10" s="12" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D10" s="13" t="inlineStr">
+      <c r="D10" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E10" s="13" t="inlineStr">
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>Luxury Segment</t>
         </is>
       </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G10" s="14" t="inlineStr">
+      <c r="F10" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G10" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H10" s="12" t="inlineStr"/>
-      <c r="I10" s="12" t="inlineStr">
+      <c r="H10" s="16" t="n">
+        <v>38.1345</v>
+      </c>
+      <c r="I10" s="13" t="inlineStr">
         <is>
           <t>989,900,000</t>
         </is>
       </c>
-      <c r="J10" s="12" t="inlineStr">
+      <c r="J10" s="13" t="inlineStr">
         <is>
           <t>770,200,000</t>
         </is>
@@ -1069,7 +1090,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H11" s="7" t="inlineStr"/>
+      <c r="H11" s="10" t="n">
+        <v>-13.7552</v>
+      </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
           <t>162,100,000</t>
@@ -1082,48 +1105,50 @@
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
-      <c r="A12" s="10" t="inlineStr">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>Swatch Group AG</t>
         </is>
       </c>
-      <c r="B12" s="11" t="inlineStr">
+      <c r="B12" s="12" t="inlineStr">
         <is>
           <t>UHR.S</t>
         </is>
       </c>
-      <c r="C12" s="12" t="inlineStr">
+      <c r="C12" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D12" s="13" t="inlineStr">
+      <c r="D12" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E12" s="13" t="inlineStr">
+      <c r="E12" s="14" t="inlineStr">
         <is>
           <t>Luxury Segment</t>
         </is>
       </c>
-      <c r="F12" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G12" s="14" t="inlineStr">
+      <c r="F12" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G12" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H12" s="12" t="inlineStr"/>
-      <c r="I12" s="12" t="inlineStr">
+      <c r="H12" s="16" t="n">
+        <v>-23.5126</v>
+      </c>
+      <c r="I12" s="13" t="inlineStr">
         <is>
           <t>306,000,000</t>
         </is>
       </c>
-      <c r="J12" s="12" t="inlineStr">
+      <c r="J12" s="13" t="inlineStr">
         <is>
           <t>1,159,000,000</t>
         </is>
@@ -1165,7 +1190,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H13" s="7" t="inlineStr"/>
+      <c r="H13" s="10" t="n">
+        <v>-10.3557</v>
+      </c>
       <c r="I13" s="7" t="inlineStr">
         <is>
           <t>162,100,000</t>
@@ -1178,48 +1205,50 @@
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
-      <c r="A14" s="10" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>Pandora A/S</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="B14" s="12" t="inlineStr">
         <is>
           <t>PNDORA.CO</t>
         </is>
       </c>
-      <c r="C14" s="12" t="inlineStr">
+      <c r="C14" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D14" s="13" t="inlineStr">
+      <c r="D14" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E14" s="13" t="inlineStr">
+      <c r="E14" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F14" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G14" s="14" t="inlineStr">
+      <c r="F14" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G14" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H14" s="12" t="inlineStr"/>
-      <c r="I14" s="12" t="inlineStr">
+      <c r="H14" s="16" t="n">
+        <v>10.4265</v>
+      </c>
+      <c r="I14" s="13" t="inlineStr">
         <is>
           <t>7,974,000,000</t>
         </is>
       </c>
-      <c r="J14" s="12" t="inlineStr">
+      <c r="J14" s="13" t="inlineStr">
         <is>
           <t>6,803,000,000</t>
         </is>
@@ -1261,7 +1290,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H15" s="7" t="inlineStr"/>
+      <c r="H15" s="10" t="n">
+        <v>-5.4254</v>
+      </c>
       <c r="I15" s="7" t="inlineStr">
         <is>
           <t>468,877,000</t>
@@ -1274,48 +1305,50 @@
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
-      <c r="A16" s="10" t="inlineStr">
+      <c r="A16" s="11" t="inlineStr">
         <is>
           <t>Potlatchdeltic Corp</t>
         </is>
       </c>
-      <c r="B16" s="11" t="inlineStr">
+      <c r="B16" s="12" t="inlineStr">
         <is>
           <t>PCH.N</t>
         </is>
       </c>
-      <c r="C16" s="12" t="inlineStr">
+      <c r="C16" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D16" s="13" t="inlineStr">
+      <c r="D16" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E16" s="13" t="inlineStr">
+      <c r="E16" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F16" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G16" s="14" t="inlineStr">
+      <c r="F16" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G16" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H16" s="12" t="inlineStr"/>
-      <c r="I16" s="12" t="inlineStr">
+      <c r="H16" s="16" t="n">
+        <v>-14.3466</v>
+      </c>
+      <c r="I16" s="13" t="inlineStr">
         <is>
           <t>120,603,000</t>
         </is>
       </c>
-      <c r="J16" s="12" t="inlineStr">
+      <c r="J16" s="13" t="inlineStr">
         <is>
           <t>477,455,000</t>
         </is>
@@ -1357,7 +1390,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H17" s="7" t="inlineStr"/>
+      <c r="H17" s="10" t="n">
+        <v>-36.8662</v>
+      </c>
       <c r="I17" s="7" t="inlineStr">
         <is>
           <t>407,625,000</t>
@@ -1370,48 +1405,50 @@
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
-      <c r="A18" s="10" t="inlineStr">
+      <c r="A18" s="11" t="inlineStr">
         <is>
           <t>Levi Strauss &amp; Co</t>
         </is>
       </c>
-      <c r="B18" s="11" t="inlineStr">
+      <c r="B18" s="12" t="inlineStr">
         <is>
           <t>LEVI.K</t>
         </is>
       </c>
-      <c r="C18" s="12" t="inlineStr">
+      <c r="C18" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D18" s="13" t="inlineStr">
+      <c r="D18" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E18" s="13" t="inlineStr">
+      <c r="E18" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F18" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G18" s="14" t="inlineStr">
+      <c r="F18" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G18" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H18" s="12" t="inlineStr"/>
-      <c r="I18" s="12" t="inlineStr">
+      <c r="H18" s="16" t="n">
+        <v>10.7013</v>
+      </c>
+      <c r="I18" s="13" t="inlineStr">
         <is>
           <t>649,900,000</t>
         </is>
       </c>
-      <c r="J18" s="12" t="inlineStr">
+      <c r="J18" s="13" t="inlineStr">
         <is>
           <t>737,300,000</t>
         </is>
@@ -1453,7 +1490,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H19" s="7" t="inlineStr"/>
+      <c r="H19" s="10" t="n">
+        <v>47.6951</v>
+      </c>
       <c r="I19" s="7" t="inlineStr">
         <is>
           <t>695,610,000</t>
@@ -1466,48 +1505,50 @@
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
-      <c r="A20" s="10" t="inlineStr">
+      <c r="A20" s="11" t="inlineStr">
         <is>
           <t>Guess? Inc</t>
         </is>
       </c>
-      <c r="B20" s="11" t="inlineStr">
+      <c r="B20" s="12" t="inlineStr">
         <is>
           <t>GES.N</t>
         </is>
       </c>
-      <c r="C20" s="12" t="inlineStr">
+      <c r="C20" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D20" s="13" t="inlineStr">
+      <c r="D20" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E20" s="13" t="inlineStr">
+      <c r="E20" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F20" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G20" s="14" t="inlineStr">
+      <c r="F20" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G20" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H20" s="12" t="inlineStr"/>
-      <c r="I20" s="12" t="inlineStr">
+      <c r="H20" s="16" t="n">
+        <v>-13.0175</v>
+      </c>
+      <c r="I20" s="13" t="inlineStr">
         <is>
           <t>179,946,000</t>
         </is>
       </c>
-      <c r="J20" s="12" t="inlineStr">
+      <c r="J20" s="13" t="inlineStr">
         <is>
           <t>255,450,000</t>
         </is>
@@ -1549,7 +1590,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H21" s="7" t="inlineStr"/>
+      <c r="H21" s="10" t="n">
+        <v>-11.4033</v>
+      </c>
       <c r="I21" s="7" t="inlineStr">
         <is>
           <t>279,428,000</t>
@@ -1562,48 +1605,50 @@
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
-      <c r="A22" s="10" t="inlineStr">
+      <c r="A22" s="11" t="inlineStr">
         <is>
           <t>HanesBrands Inc</t>
         </is>
       </c>
-      <c r="B22" s="11" t="inlineStr">
+      <c r="B22" s="12" t="inlineStr">
         <is>
           <t>HBI</t>
         </is>
       </c>
-      <c r="C22" s="12" t="inlineStr">
+      <c r="C22" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D22" s="13" t="inlineStr">
+      <c r="D22" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E22" s="13" t="inlineStr">
+      <c r="E22" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F22" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G22" s="14" t="inlineStr">
+      <c r="F22" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G22" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H22" s="12" t="inlineStr"/>
-      <c r="I22" s="12" t="inlineStr">
+      <c r="H22" s="16" t="n">
+        <v>58.7444</v>
+      </c>
+      <c r="I22" s="13" t="inlineStr">
         <is>
           <t>415,171,000</t>
         </is>
       </c>
-      <c r="J22" s="12" t="inlineStr">
+      <c r="J22" s="13" t="inlineStr">
         <is>
           <t>322,013,000</t>
         </is>
@@ -1645,7 +1690,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H23" s="7" t="inlineStr"/>
+      <c r="H23" s="10" t="n">
+        <v>-25.0484</v>
+      </c>
       <c r="I23" s="7" t="inlineStr">
         <is>
           <t>624,200,000</t>
@@ -1658,48 +1705,50 @@
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
-      <c r="A24" s="10" t="inlineStr">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t>Kontoor Brands Inc</t>
         </is>
       </c>
-      <c r="B24" s="11" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t>KTB</t>
         </is>
       </c>
-      <c r="C24" s="12" t="inlineStr">
+      <c r="C24" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D24" s="13" t="inlineStr">
+      <c r="D24" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E24" s="13" t="inlineStr">
+      <c r="E24" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F24" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G24" s="14" t="inlineStr">
+      <c r="F24" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G24" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H24" s="12" t="inlineStr"/>
-      <c r="I24" s="12" t="inlineStr">
+      <c r="H24" s="16" t="n">
+        <v>25.4406</v>
+      </c>
+      <c r="I24" s="13" t="inlineStr">
         <is>
           <t>382,289,000</t>
         </is>
       </c>
-      <c r="J24" s="12" t="inlineStr">
+      <c r="J24" s="13" t="inlineStr">
         <is>
           <t>356,665,000</t>
         </is>
@@ -1741,7 +1790,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H25" s="7" t="inlineStr"/>
+      <c r="H25" s="10" t="n">
+        <v>-23.8843</v>
+      </c>
       <c r="I25" s="7" t="inlineStr">
         <is>
           <t>200,000,000</t>
@@ -1754,48 +1805,48 @@
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
-      <c r="A26" s="10" t="inlineStr">
+      <c r="A26" s="11" t="inlineStr">
         <is>
           <t>Oxford Industries Inc</t>
         </is>
       </c>
-      <c r="B26" s="11" t="inlineStr">
+      <c r="B26" s="12" t="inlineStr">
         <is>
           <t>OXM</t>
         </is>
       </c>
-      <c r="C26" s="12" t="inlineStr">
+      <c r="C26" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D26" s="13" t="inlineStr">
+      <c r="D26" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E26" s="13" t="inlineStr">
+      <c r="E26" s="14" t="inlineStr">
         <is>
           <t>Affordable Segment</t>
         </is>
       </c>
-      <c r="F26" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G26" s="14" t="inlineStr">
+      <c r="F26" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G26" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H26" s="12" t="inlineStr"/>
-      <c r="I26" s="12" t="inlineStr">
+      <c r="H26" s="13" t="inlineStr"/>
+      <c r="I26" s="13" t="inlineStr">
         <is>
           <t>125,386,000</t>
         </is>
       </c>
-      <c r="J26" s="12" t="inlineStr">
+      <c r="J26" s="13" t="inlineStr">
         <is>
           <t>222,557,000</t>
         </is>
@@ -1837,7 +1888,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H27" s="7" t="inlineStr"/>
+      <c r="H27" s="10" t="n">
+        <v>3.4884</v>
+      </c>
       <c r="I27" s="7" t="inlineStr">
         <is>
           <t>360,803,535,170</t>
@@ -1850,48 +1903,50 @@
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
-      <c r="A28" s="10" t="inlineStr">
+      <c r="A28" s="11" t="inlineStr">
         <is>
           <t>Columbia Sportswear Co</t>
         </is>
       </c>
-      <c r="B28" s="11" t="inlineStr">
+      <c r="B28" s="12" t="inlineStr">
         <is>
           <t>COLM.O</t>
         </is>
       </c>
-      <c r="C28" s="12" t="inlineStr">
+      <c r="C28" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D28" s="13" t="inlineStr">
+      <c r="D28" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E28" s="13" t="inlineStr">
+      <c r="E28" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F28" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G28" s="14" t="inlineStr">
+      <c r="F28" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G28" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H28" s="12" t="inlineStr"/>
-      <c r="I28" s="12" t="inlineStr">
+      <c r="H28" s="17" t="n">
+        <v>-0.5531</v>
+      </c>
+      <c r="I28" s="13" t="inlineStr">
         <is>
           <t>270,741,000</t>
         </is>
       </c>
-      <c r="J28" s="12" t="inlineStr">
+      <c r="J28" s="13" t="inlineStr">
         <is>
           <t>429,504,000</t>
         </is>
@@ -1933,7 +1988,9 @@
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H29" s="7" t="inlineStr"/>
+      <c r="H29" s="10" t="n">
+        <v>2.0478</v>
+      </c>
       <c r="I29" s="7" t="inlineStr">
         <is>
           <t>202,146,000</t>
@@ -1946,48 +2003,48 @@
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
-      <c r="A30" s="10" t="inlineStr">
+      <c r="A30" s="11" t="inlineStr">
         <is>
           <t>Amer Sports Inc</t>
         </is>
       </c>
-      <c r="B30" s="11" t="inlineStr">
+      <c r="B30" s="12" t="inlineStr">
         <is>
           <t>AS</t>
         </is>
       </c>
-      <c r="C30" s="12" t="inlineStr">
+      <c r="C30" s="13" t="inlineStr">
         <is>
           <t>Consumer Discretionary</t>
         </is>
       </c>
-      <c r="D30" s="13" t="inlineStr">
+      <c r="D30" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E30" s="13" t="inlineStr">
+      <c r="E30" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F30" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G30" s="14" t="inlineStr">
+      <c r="F30" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G30" s="15" t="inlineStr">
         <is>
           <t>Zeile 1</t>
         </is>
       </c>
-      <c r="H30" s="12" t="inlineStr"/>
-      <c r="I30" s="12" t="inlineStr">
+      <c r="H30" s="13" t="inlineStr"/>
+      <c r="I30" s="13" t="inlineStr">
         <is>
           <t>520,100,000</t>
         </is>
       </c>
-      <c r="J30" s="12" t="inlineStr">
+      <c r="J30" s="13" t="inlineStr">
         <is>
           <t>252,000,000</t>
         </is>
@@ -2029,7 +2086,9 @@
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H31" s="7" t="inlineStr"/>
+      <c r="H31" s="10" t="n">
+        <v>-2.4463</v>
+      </c>
       <c r="I31" s="7" t="inlineStr">
         <is>
           <t>14,724,000,000</t>
@@ -2042,48 +2101,50 @@
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
-      <c r="A32" s="10" t="inlineStr">
+      <c r="A32" s="11" t="inlineStr">
         <is>
           <t>Keurig Dr Pepper Inc</t>
         </is>
       </c>
-      <c r="B32" s="11" t="inlineStr">
+      <c r="B32" s="12" t="inlineStr">
         <is>
           <t>KDP.O</t>
         </is>
       </c>
-      <c r="C32" s="12" t="inlineStr">
+      <c r="C32" s="13" t="inlineStr">
         <is>
           <t>Consumer Staples</t>
         </is>
       </c>
-      <c r="D32" s="13" t="inlineStr">
+      <c r="D32" s="14" t="inlineStr">
         <is>
           <t>Soft Drinks</t>
         </is>
       </c>
-      <c r="E32" s="13" t="inlineStr">
+      <c r="E32" s="14" t="inlineStr">
         <is>
           <t>Beverages</t>
         </is>
       </c>
-      <c r="F32" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G32" s="14" t="inlineStr">
+      <c r="F32" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G32" s="15" t="inlineStr">
         <is>
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H32" s="12" t="inlineStr"/>
-      <c r="I32" s="12" t="inlineStr">
+      <c r="H32" s="16" t="n">
+        <v>3.0822</v>
+      </c>
+      <c r="I32" s="13" t="inlineStr">
         <is>
           <t>3,400,000,000</t>
         </is>
       </c>
-      <c r="J32" s="12" t="inlineStr">
+      <c r="J32" s="13" t="inlineStr">
         <is>
           <t>2,983,000,000</t>
         </is>
@@ -2125,7 +2186,9 @@
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H33" s="7" t="inlineStr"/>
+      <c r="H33" s="10" t="n">
+        <v>10.3658</v>
+      </c>
       <c r="I33" s="7" t="inlineStr">
         <is>
           <t>68,953,000,000</t>
@@ -2138,48 +2201,50 @@
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
-      <c r="A34" s="10" t="inlineStr">
+      <c r="A34" s="11" t="inlineStr">
         <is>
           <t>Coca-Cola Europacific Partners PLC</t>
         </is>
       </c>
-      <c r="B34" s="11" t="inlineStr">
+      <c r="B34" s="12" t="inlineStr">
         <is>
           <t>CCEP.O</t>
         </is>
       </c>
-      <c r="C34" s="12" t="inlineStr">
+      <c r="C34" s="13" t="inlineStr">
         <is>
           <t>Consumer Staples</t>
         </is>
       </c>
-      <c r="D34" s="13" t="inlineStr">
+      <c r="D34" s="14" t="inlineStr">
         <is>
           <t>Soft Drinks</t>
         </is>
       </c>
-      <c r="E34" s="13" t="inlineStr">
+      <c r="E34" s="14" t="inlineStr">
         <is>
           <t>Beverages</t>
         </is>
       </c>
-      <c r="F34" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G34" s="14" t="inlineStr">
+      <c r="F34" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G34" s="15" t="inlineStr">
         <is>
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H34" s="12" t="inlineStr"/>
-      <c r="I34" s="12" t="inlineStr">
+      <c r="H34" s="16" t="n">
+        <v>7.1215</v>
+      </c>
+      <c r="I34" s="13" t="inlineStr">
         <is>
           <t>2,614,000,000</t>
         </is>
       </c>
-      <c r="J34" s="12" t="inlineStr">
+      <c r="J34" s="13" t="inlineStr">
         <is>
           <t>2,324,000,000</t>
         </is>
@@ -2221,7 +2286,9 @@
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H35" s="7" t="inlineStr"/>
+      <c r="H35" s="10" t="n">
+        <v>3.3866</v>
+      </c>
       <c r="I35" s="7" t="inlineStr">
         <is>
           <t>2,069,094,000</t>
@@ -2234,48 +2301,50 @@
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
-      <c r="A36" s="10" t="inlineStr">
+      <c r="A36" s="11" t="inlineStr">
         <is>
           <t>Arca Continental SAB de CV</t>
         </is>
       </c>
-      <c r="B36" s="11" t="inlineStr">
+      <c r="B36" s="12" t="inlineStr">
         <is>
           <t>AC.MX</t>
         </is>
       </c>
-      <c r="C36" s="12" t="inlineStr">
+      <c r="C36" s="13" t="inlineStr">
         <is>
           <t>Consumer Staples</t>
         </is>
       </c>
-      <c r="D36" s="13" t="inlineStr">
+      <c r="D36" s="14" t="inlineStr">
         <is>
           <t>Soft Drinks</t>
         </is>
       </c>
-      <c r="E36" s="13" t="inlineStr">
+      <c r="E36" s="14" t="inlineStr">
         <is>
           <t>Beverages</t>
         </is>
       </c>
-      <c r="F36" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G36" s="14" t="inlineStr">
+      <c r="F36" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G36" s="15" t="inlineStr">
         <is>
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H36" s="12" t="inlineStr"/>
-      <c r="I36" s="12" t="inlineStr">
+      <c r="H36" s="16" t="n">
+        <v>22.8146</v>
+      </c>
+      <c r="I36" s="13" t="inlineStr">
         <is>
           <t>39,190,682,000</t>
         </is>
       </c>
-      <c r="J36" s="12" t="inlineStr">
+      <c r="J36" s="13" t="inlineStr">
         <is>
           <t>30,691,220,000</t>
         </is>
@@ -2317,7 +2386,9 @@
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H37" s="7" t="inlineStr"/>
+      <c r="H37" s="10" t="n">
+        <v>24.0117</v>
+      </c>
       <c r="I37" s="7" t="inlineStr">
         <is>
           <t>1,194,000,000</t>
@@ -2330,48 +2401,50 @@
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
-      <c r="A38" s="10" t="inlineStr">
+      <c r="A38" s="11" t="inlineStr">
         <is>
           <t>Suntory Beverage &amp; Food Ltd</t>
         </is>
       </c>
-      <c r="B38" s="11" t="inlineStr">
+      <c r="B38" s="12" t="inlineStr">
         <is>
           <t>2587.T</t>
         </is>
       </c>
-      <c r="C38" s="12" t="inlineStr">
+      <c r="C38" s="13" t="inlineStr">
         <is>
           <t>Consumer Staples</t>
         </is>
       </c>
-      <c r="D38" s="13" t="inlineStr">
+      <c r="D38" s="14" t="inlineStr">
         <is>
           <t>Soft Drinks</t>
         </is>
       </c>
-      <c r="E38" s="13" t="inlineStr">
+      <c r="E38" s="14" t="inlineStr">
         <is>
           <t>Beverages</t>
         </is>
       </c>
-      <c r="F38" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G38" s="14" t="inlineStr">
+      <c r="F38" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G38" s="15" t="inlineStr">
         <is>
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H38" s="12" t="inlineStr"/>
-      <c r="I38" s="12" t="inlineStr">
+      <c r="H38" s="16" t="n">
+        <v>-3.5507</v>
+      </c>
+      <c r="I38" s="13" t="inlineStr">
         <is>
           <t>169,975,000,000</t>
         </is>
       </c>
-      <c r="J38" s="12" t="inlineStr">
+      <c r="J38" s="13" t="inlineStr">
         <is>
           <t>133,783,000,000</t>
         </is>
@@ -2426,48 +2499,48 @@
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
-      <c r="A40" s="10" t="inlineStr">
+      <c r="A40" s="11" t="inlineStr">
         <is>
           <t>Primo Water Corp</t>
         </is>
       </c>
-      <c r="B40" s="11" t="inlineStr">
+      <c r="B40" s="12" t="inlineStr">
         <is>
           <t>PRMW.TO</t>
         </is>
       </c>
-      <c r="C40" s="12" t="inlineStr">
+      <c r="C40" s="13" t="inlineStr">
         <is>
           <t>Consumer Staples</t>
         </is>
       </c>
-      <c r="D40" s="13" t="inlineStr">
+      <c r="D40" s="14" t="inlineStr">
         <is>
           <t>Soft Drinks</t>
         </is>
       </c>
-      <c r="E40" s="13" t="inlineStr">
+      <c r="E40" s="14" t="inlineStr">
         <is>
           <t>Beverages</t>
         </is>
       </c>
-      <c r="F40" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G40" s="14" t="inlineStr">
+      <c r="F40" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G40" s="15" t="inlineStr">
         <is>
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H40" s="12" t="inlineStr"/>
-      <c r="I40" s="12" t="inlineStr">
+      <c r="H40" s="13" t="inlineStr"/>
+      <c r="I40" s="13" t="inlineStr">
         <is>
           <t>161,000,000</t>
         </is>
       </c>
-      <c r="J40" s="12" t="inlineStr">
+      <c r="J40" s="13" t="inlineStr">
         <is>
           <t>121,800,000</t>
         </is>
@@ -2509,7 +2582,9 @@
           <t>Zeile 2</t>
         </is>
       </c>
-      <c r="H41" s="7" t="inlineStr"/>
+      <c r="H41" s="10" t="n">
+        <v>-4.898</v>
+      </c>
       <c r="I41" s="7" t="inlineStr">
         <is>
           <t>235,459,000</t>
@@ -2522,48 +2597,46 @@
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
-      <c r="A42" s="10" t="inlineStr">
+      <c r="A42" s="11" t="inlineStr">
         <is>
           <t>Scout24 SE</t>
         </is>
       </c>
-      <c r="B42" s="11" t="inlineStr">
+      <c r="B42" s="12" t="inlineStr">
         <is>
           <t>RMV.L</t>
         </is>
       </c>
-      <c r="C42" s="12" t="inlineStr">
+      <c r="C42" s="13" t="inlineStr">
         <is>
           <t>Real Estate</t>
         </is>
       </c>
-      <c r="D42" s="13" t="inlineStr">
+      <c r="D42" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E42" s="13" t="inlineStr">
+      <c r="E42" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F42" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G42" s="14" t="inlineStr">
+      <c r="F42" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G42" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H42" s="12" t="inlineStr"/>
-      <c r="I42" s="12" t="inlineStr">
-        <is>
-          <t>265,560,000</t>
-        </is>
-      </c>
-      <c r="J42" s="12" t="inlineStr">
+      <c r="H42" s="16" t="n">
+        <v>17.3732</v>
+      </c>
+      <c r="I42" s="13" t="inlineStr"/>
+      <c r="J42" s="13" t="inlineStr">
         <is>
           <t>241,343,000</t>
         </is>
@@ -2606,11 +2679,7 @@
         </is>
       </c>
       <c r="H43" s="7" t="inlineStr"/>
-      <c r="I43" s="7" t="inlineStr">
-        <is>
-          <t>93,250,000</t>
-        </is>
-      </c>
+      <c r="I43" s="7" t="inlineStr"/>
       <c r="J43" s="7" t="inlineStr">
         <is>
           <t>84,455,000</t>
@@ -2618,48 +2687,46 @@
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
-      <c r="A44" s="10" t="inlineStr">
+      <c r="A44" s="11" t="inlineStr">
         <is>
           <t>Meta Platforms Inc</t>
         </is>
       </c>
-      <c r="B44" s="11" t="inlineStr">
+      <c r="B44" s="12" t="inlineStr">
         <is>
           <t>META.O</t>
         </is>
       </c>
-      <c r="C44" s="12" t="inlineStr">
+      <c r="C44" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D44" s="13" t="inlineStr">
+      <c r="D44" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E44" s="13" t="inlineStr">
+      <c r="E44" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F44" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G44" s="14" t="inlineStr">
+      <c r="F44" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G44" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H44" s="12" t="inlineStr"/>
-      <c r="I44" s="12" t="inlineStr">
-        <is>
-          <t>69,769,000,000</t>
-        </is>
-      </c>
-      <c r="J44" s="12" t="inlineStr">
+      <c r="H44" s="16" t="n">
+        <v>78.2094</v>
+      </c>
+      <c r="I44" s="13" t="inlineStr"/>
+      <c r="J44" s="13" t="inlineStr">
         <is>
           <t>33,555,000,000</t>
         </is>
@@ -2701,60 +2768,56 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H45" s="7" t="inlineStr"/>
-      <c r="I45" s="15" t="inlineStr">
-        <is>
-          <t>-717137000.00</t>
-        </is>
-      </c>
-      <c r="J45" s="15" t="inlineStr">
+      <c r="H45" s="10" t="n">
+        <v>-32.7819</v>
+      </c>
+      <c r="I45" s="7" t="inlineStr"/>
+      <c r="J45" s="10" t="inlineStr">
         <is>
           <t>-1206357000.00</t>
         </is>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
-      <c r="A46" s="10" t="inlineStr">
+      <c r="A46" s="11" t="inlineStr">
         <is>
           <t>Pinterest Inc</t>
         </is>
       </c>
-      <c r="B46" s="11" t="inlineStr">
+      <c r="B46" s="12" t="inlineStr">
         <is>
           <t>PINS.N</t>
         </is>
       </c>
-      <c r="C46" s="12" t="inlineStr">
+      <c r="C46" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D46" s="13" t="inlineStr">
+      <c r="D46" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E46" s="13" t="inlineStr">
+      <c r="E46" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F46" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G46" s="14" t="inlineStr">
+      <c r="F46" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G46" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H46" s="12" t="inlineStr"/>
-      <c r="I46" s="12" t="inlineStr">
-        <is>
-          <t>214,467,000</t>
-        </is>
-      </c>
+      <c r="H46" s="16" t="n">
+        <v>-16.7386</v>
+      </c>
+      <c r="I46" s="13" t="inlineStr"/>
       <c r="J46" s="16" t="inlineStr">
         <is>
           <t>-81177000.00</t>
@@ -2797,12 +2860,10 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H47" s="7" t="inlineStr"/>
-      <c r="I47" s="7" t="inlineStr">
-        <is>
-          <t>208,154,000,000</t>
-        </is>
-      </c>
+      <c r="H47" s="10" t="n">
+        <v>39.5095</v>
+      </c>
+      <c r="I47" s="7" t="inlineStr"/>
       <c r="J47" s="7" t="inlineStr">
         <is>
           <t>106,358,000,000</t>
@@ -2810,48 +2871,46 @@
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
-      <c r="A48" s="10" t="inlineStr">
+      <c r="A48" s="11" t="inlineStr">
         <is>
           <t>Naver Corp</t>
         </is>
       </c>
-      <c r="B48" s="11" t="inlineStr">
+      <c r="B48" s="12" t="inlineStr">
         <is>
           <t>035420.KS</t>
         </is>
       </c>
-      <c r="C48" s="12" t="inlineStr">
+      <c r="C48" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D48" s="13" t="inlineStr">
+      <c r="D48" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E48" s="13" t="inlineStr">
+      <c r="E48" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F48" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G48" s="14" t="inlineStr">
+      <c r="F48" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G48" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H48" s="12" t="inlineStr"/>
-      <c r="I48" s="12" t="inlineStr">
-        <is>
-          <t>1,979,263,438,830</t>
-        </is>
-      </c>
-      <c r="J48" s="12" t="inlineStr">
+      <c r="H48" s="16" t="n">
+        <v>-6.2499</v>
+      </c>
+      <c r="I48" s="13" t="inlineStr"/>
+      <c r="J48" s="13" t="inlineStr">
         <is>
           <t>1,304,664,410,540</t>
         </is>
@@ -2893,12 +2952,10 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H49" s="7" t="inlineStr"/>
-      <c r="I49" s="7" t="inlineStr">
-        <is>
-          <t>460,212,161,530</t>
-        </is>
-      </c>
+      <c r="H49" s="10" t="n">
+        <v>-15.4695</v>
+      </c>
+      <c r="I49" s="7" t="inlineStr"/>
       <c r="J49" s="7" t="inlineStr">
         <is>
           <t>569,390,445,170</t>
@@ -2906,48 +2963,46 @@
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
-      <c r="A50" s="10" t="inlineStr">
+      <c r="A50" s="11" t="inlineStr">
         <is>
           <t>Baidu Inc</t>
         </is>
       </c>
-      <c r="B50" s="11" t="inlineStr">
+      <c r="B50" s="12" t="inlineStr">
         <is>
           <t>BIDU.O</t>
         </is>
       </c>
-      <c r="C50" s="12" t="inlineStr">
+      <c r="C50" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D50" s="13" t="inlineStr">
+      <c r="D50" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E50" s="13" t="inlineStr">
+      <c r="E50" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F50" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G50" s="14" t="inlineStr">
+      <c r="F50" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G50" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H50" s="12" t="inlineStr"/>
-      <c r="I50" s="12" t="inlineStr">
-        <is>
-          <t>21,270,000,000</t>
-        </is>
-      </c>
-      <c r="J50" s="12" t="inlineStr">
+      <c r="H50" s="16" t="n">
+        <v>-24.1581</v>
+      </c>
+      <c r="I50" s="13" t="inlineStr"/>
+      <c r="J50" s="13" t="inlineStr">
         <is>
           <t>15,912,000,000</t>
         </is>
@@ -2989,12 +3044,10 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H51" s="7" t="inlineStr"/>
-      <c r="I51" s="7" t="inlineStr">
-        <is>
-          <t>853,912,000</t>
-        </is>
-      </c>
+      <c r="H51" s="10" t="n">
+        <v>-16.2191</v>
+      </c>
+      <c r="I51" s="7" t="inlineStr"/>
       <c r="J51" s="7" t="inlineStr">
         <is>
           <t>515,005,000</t>
@@ -3002,48 +3055,46 @@
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
-      <c r="A52" s="10" t="inlineStr">
+      <c r="A52" s="11" t="inlineStr">
         <is>
           <t>LY Corp</t>
         </is>
       </c>
-      <c r="B52" s="11" t="inlineStr">
+      <c r="B52" s="12" t="inlineStr">
         <is>
           <t>4689.T</t>
         </is>
       </c>
-      <c r="C52" s="12" t="inlineStr">
+      <c r="C52" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D52" s="13" t="inlineStr">
+      <c r="D52" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E52" s="13" t="inlineStr">
+      <c r="E52" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F52" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G52" s="14" t="inlineStr">
+      <c r="F52" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G52" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H52" s="12" t="inlineStr"/>
-      <c r="I52" s="12" t="inlineStr">
-        <is>
-          <t>271,978,000,000</t>
-        </is>
-      </c>
-      <c r="J52" s="12" t="inlineStr">
+      <c r="H52" s="16" t="n">
+        <v>-11.7269</v>
+      </c>
+      <c r="I52" s="13" t="inlineStr"/>
+      <c r="J52" s="13" t="inlineStr">
         <is>
           <t>159,365,000,000</t>
         </is>
@@ -3085,12 +3136,10 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H53" s="7" t="inlineStr"/>
-      <c r="I53" s="7" t="inlineStr">
-        <is>
-          <t>198,921,000</t>
-        </is>
-      </c>
+      <c r="H53" s="10" t="n">
+        <v>-12.2785</v>
+      </c>
+      <c r="I53" s="7" t="inlineStr"/>
       <c r="J53" s="7" t="inlineStr">
         <is>
           <t>226,310,000</t>
@@ -3098,48 +3147,46 @@
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
-      <c r="A54" s="10" t="inlineStr">
+      <c r="A54" s="11" t="inlineStr">
         <is>
           <t>Yelp Inc</t>
         </is>
       </c>
-      <c r="B54" s="11" t="inlineStr">
+      <c r="B54" s="12" t="inlineStr">
         <is>
           <t>YELP.K</t>
         </is>
       </c>
-      <c r="C54" s="12" t="inlineStr">
+      <c r="C54" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D54" s="13" t="inlineStr">
+      <c r="D54" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E54" s="13" t="inlineStr">
+      <c r="E54" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F54" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G54" s="14" t="inlineStr">
+      <c r="F54" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G54" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H54" s="12" t="inlineStr"/>
-      <c r="I54" s="12" t="inlineStr">
-        <is>
-          <t>158,225,000</t>
-        </is>
-      </c>
-      <c r="J54" s="12" t="inlineStr">
+      <c r="H54" s="16" t="n">
+        <v>-15.1034</v>
+      </c>
+      <c r="I54" s="13" t="inlineStr"/>
+      <c r="J54" s="13" t="inlineStr">
         <is>
           <t>68,817,000</t>
         </is>
@@ -3181,12 +3228,10 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H55" s="7" t="inlineStr"/>
-      <c r="I55" s="7" t="inlineStr">
-        <is>
-          <t>474,627,000</t>
-        </is>
-      </c>
+      <c r="H55" s="10" t="n">
+        <v>22.4149</v>
+      </c>
+      <c r="I55" s="7" t="inlineStr"/>
       <c r="J55" s="7" t="inlineStr">
         <is>
           <t>353,622,000</t>
@@ -3194,48 +3239,46 @@
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
-      <c r="A56" s="10" t="inlineStr">
+      <c r="A56" s="11" t="inlineStr">
         <is>
           <t>REA Group Ltd</t>
         </is>
       </c>
-      <c r="B56" s="11" t="inlineStr">
+      <c r="B56" s="12" t="inlineStr">
         <is>
           <t>REA.AX</t>
         </is>
       </c>
-      <c r="C56" s="12" t="inlineStr">
+      <c r="C56" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D56" s="13" t="inlineStr">
+      <c r="D56" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E56" s="13" t="inlineStr">
+      <c r="E56" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F56" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G56" s="14" t="inlineStr">
+      <c r="F56" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G56" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H56" s="12" t="inlineStr"/>
-      <c r="I56" s="12" t="inlineStr">
-        <is>
-          <t>820,700,000</t>
-        </is>
-      </c>
-      <c r="J56" s="12" t="inlineStr">
+      <c r="H56" s="16" t="n">
+        <v>33.1493</v>
+      </c>
+      <c r="I56" s="13" t="inlineStr"/>
+      <c r="J56" s="13" t="inlineStr">
         <is>
           <t>560,700,000</t>
         </is>
@@ -3277,53 +3320,53 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H57" s="7" t="inlineStr"/>
+      <c r="H57" s="10" t="n">
+        <v>-42.6175</v>
+      </c>
       <c r="I57" s="7" t="inlineStr"/>
       <c r="J57" s="7" t="inlineStr"/>
     </row>
     <row r="58" ht="20" customHeight="1">
-      <c r="A58" s="10" t="inlineStr">
+      <c r="A58" s="11" t="inlineStr">
         <is>
           <t>Tripadvisor Inc</t>
         </is>
       </c>
-      <c r="B58" s="11" t="inlineStr">
+      <c r="B58" s="12" t="inlineStr">
         <is>
           <t>TRIP.OQ</t>
         </is>
       </c>
-      <c r="C58" s="12" t="inlineStr">
+      <c r="C58" s="13" t="inlineStr">
         <is>
           <t>Information Technology</t>
         </is>
       </c>
-      <c r="D58" s="13" t="inlineStr">
+      <c r="D58" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E58" s="13" t="inlineStr">
+      <c r="E58" s="14" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="F58" s="14" t="inlineStr">
-        <is>
-          <t>Sub-Industry</t>
-        </is>
-      </c>
-      <c r="G58" s="14" t="inlineStr">
+      <c r="F58" s="15" t="inlineStr">
+        <is>
+          <t>Sub-Industry</t>
+        </is>
+      </c>
+      <c r="G58" s="15" t="inlineStr">
         <is>
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H58" s="12" t="inlineStr"/>
-      <c r="I58" s="12" t="inlineStr">
-        <is>
-          <t>134,000,000</t>
-        </is>
-      </c>
-      <c r="J58" s="12" t="inlineStr">
+      <c r="H58" s="16" t="n">
+        <v>-36.5071</v>
+      </c>
+      <c r="I58" s="13" t="inlineStr"/>
+      <c r="J58" s="13" t="inlineStr">
         <is>
           <t>98,000,000</t>
         </is>
@@ -3365,12 +3408,10 @@
           <t>Zeile 3</t>
         </is>
       </c>
-      <c r="H59" s="7" t="inlineStr"/>
-      <c r="I59" s="15" t="inlineStr">
-        <is>
-          <t>-2003000.00</t>
-        </is>
-      </c>
+      <c r="H59" s="10" t="n">
+        <v>-2.4589</v>
+      </c>
+      <c r="I59" s="7" t="inlineStr"/>
       <c r="J59" s="7" t="inlineStr">
         <is>
           <t>85,980,000</t>
@@ -3378,26 +3419,26 @@
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
-      <c r="A60" s="10" t="inlineStr">
+      <c r="A60" s="11" t="inlineStr">
         <is>
           <t>💼 Ø Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="B60" s="11" t="inlineStr"/>
-      <c r="C60" s="12" t="inlineStr"/>
-      <c r="D60" s="13" t="inlineStr">
+      <c r="B60" s="12" t="inlineStr"/>
+      <c r="C60" s="13" t="inlineStr"/>
+      <c r="D60" s="14" t="inlineStr">
         <is>
           <t>Apparel, Accessories &amp; Luxury Goods</t>
         </is>
       </c>
-      <c r="E60" s="13" t="inlineStr"/>
-      <c r="F60" s="14" t="inlineStr"/>
-      <c r="G60" s="14" t="inlineStr"/>
+      <c r="E60" s="14" t="inlineStr"/>
+      <c r="F60" s="15" t="inlineStr"/>
+      <c r="G60" s="15" t="inlineStr"/>
       <c r="H60" s="16" t="n">
         <v>-4.415934615384616</v>
       </c>
-      <c r="I60" s="12" t="inlineStr"/>
-      <c r="J60" s="12" t="inlineStr"/>
+      <c r="I60" s="13" t="inlineStr"/>
+      <c r="J60" s="13" t="inlineStr"/>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" s="5" t="inlineStr">
@@ -3415,33 +3456,33 @@
       <c r="E61" s="8" t="inlineStr"/>
       <c r="F61" s="9" t="inlineStr"/>
       <c r="G61" s="9" t="inlineStr"/>
-      <c r="H61" s="15" t="n">
+      <c r="H61" s="10" t="n">
         <v>6.654155555555556</v>
       </c>
       <c r="I61" s="7" t="inlineStr"/>
       <c r="J61" s="7" t="inlineStr"/>
     </row>
     <row r="62" ht="20" customHeight="1">
-      <c r="A62" s="10" t="inlineStr">
+      <c r="A62" s="11" t="inlineStr">
         <is>
           <t>💼 Ø Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="B62" s="11" t="inlineStr"/>
-      <c r="C62" s="12" t="inlineStr"/>
-      <c r="D62" s="13" t="inlineStr">
+      <c r="B62" s="12" t="inlineStr"/>
+      <c r="C62" s="13" t="inlineStr"/>
+      <c r="D62" s="14" t="inlineStr">
         <is>
           <t>Interactive Media &amp; Services</t>
         </is>
       </c>
-      <c r="E62" s="13" t="inlineStr"/>
-      <c r="F62" s="14" t="inlineStr"/>
-      <c r="G62" s="14" t="inlineStr"/>
+      <c r="E62" s="14" t="inlineStr"/>
+      <c r="F62" s="15" t="inlineStr"/>
+      <c r="G62" s="15" t="inlineStr"/>
       <c r="H62" s="16" t="n">
         <v>2.359633333333333</v>
       </c>
-      <c r="I62" s="12" t="inlineStr"/>
-      <c r="J62" s="12" t="inlineStr"/>
+      <c r="I62" s="13" t="inlineStr"/>
+      <c r="J62" s="13" t="inlineStr"/>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" s="5" t="inlineStr">
@@ -3467,32 +3508,32 @@
           <t>Focus-Ø (7 Unternehmen)</t>
         </is>
       </c>
-      <c r="H63" s="15" t="n">
+      <c r="H63" s="10" t="n">
         <v>-19.04637142857143</v>
       </c>
       <c r="I63" s="7" t="inlineStr"/>
       <c r="J63" s="7" t="inlineStr"/>
     </row>
     <row r="64" ht="20" customHeight="1">
-      <c r="A64" s="10" t="inlineStr">
+      <c r="A64" s="11" t="inlineStr">
         <is>
           <t>🎯 Ø Luxury Segment</t>
         </is>
       </c>
-      <c r="B64" s="11" t="inlineStr"/>
-      <c r="C64" s="12" t="inlineStr"/>
-      <c r="D64" s="13" t="inlineStr"/>
-      <c r="E64" s="13" t="inlineStr">
+      <c r="B64" s="12" t="inlineStr"/>
+      <c r="C64" s="13" t="inlineStr"/>
+      <c r="D64" s="14" t="inlineStr"/>
+      <c r="E64" s="14" t="inlineStr">
         <is>
           <t>Luxury Segment</t>
         </is>
       </c>
-      <c r="F64" s="14" t="inlineStr">
+      <c r="F64" s="15" t="inlineStr">
         <is>
           <t>Focus-Durchschnitt</t>
         </is>
       </c>
-      <c r="G64" s="14" t="inlineStr">
+      <c r="G64" s="15" t="inlineStr">
         <is>
           <t>Focus-Ø (4 Unternehmen)</t>
         </is>
@@ -3500,8 +3541,8 @@
       <c r="H64" s="16" t="n">
         <v>-2.37225</v>
       </c>
-      <c r="I64" s="12" t="inlineStr"/>
-      <c r="J64" s="12" t="inlineStr"/>
+      <c r="I64" s="13" t="inlineStr"/>
+      <c r="J64" s="13" t="inlineStr"/>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" s="5" t="inlineStr">
@@ -3527,32 +3568,32 @@
           <t>Focus-Ø (12 Unternehmen)</t>
         </is>
       </c>
-      <c r="H65" s="15" t="n">
+      <c r="H65" s="10" t="n">
         <v>1.918016666666666</v>
       </c>
       <c r="I65" s="7" t="inlineStr"/>
       <c r="J65" s="7" t="inlineStr"/>
     </row>
     <row r="66" ht="20" customHeight="1">
-      <c r="A66" s="10" t="inlineStr">
+      <c r="A66" s="11" t="inlineStr">
         <is>
           <t>🎯 Ø Beverages</t>
         </is>
       </c>
-      <c r="B66" s="11" t="inlineStr"/>
-      <c r="C66" s="12" t="inlineStr"/>
-      <c r="D66" s="13" t="inlineStr"/>
-      <c r="E66" s="13" t="inlineStr">
+      <c r="B66" s="12" t="inlineStr"/>
+      <c r="C66" s="13" t="inlineStr"/>
+      <c r="D66" s="14" t="inlineStr"/>
+      <c r="E66" s="14" t="inlineStr">
         <is>
           <t>Beverages</t>
         </is>
       </c>
-      <c r="F66" s="14" t="inlineStr">
+      <c r="F66" s="15" t="inlineStr">
         <is>
           <t>Focus-Durchschnitt</t>
         </is>
       </c>
-      <c r="G66" s="14" t="inlineStr">
+      <c r="G66" s="15" t="inlineStr">
         <is>
           <t>Focus-Ø (11 Unternehmen)</t>
         </is>
@@ -3560,8 +3601,8 @@
       <c r="H66" s="16" t="n">
         <v>6.654155555555556</v>
       </c>
-      <c r="I66" s="12" t="inlineStr"/>
-      <c r="J66" s="12" t="inlineStr"/>
+      <c r="I66" s="13" t="inlineStr"/>
+      <c r="J66" s="13" t="inlineStr"/>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" s="5" t="inlineStr">
@@ -3588,43 +3629,43 @@
         </is>
       </c>
       <c r="H67" s="7" t="inlineStr"/>
-      <c r="I67" s="15" t="n">
-        <v>630361361.9697</v>
-      </c>
-      <c r="J67" s="15" t="n">
-        <v>749236609.6895</v>
+      <c r="I67" s="10" t="n">
+        <v>633053920.7848001</v>
+      </c>
+      <c r="J67" s="10" t="n">
+        <v>752977042.0763</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
-      <c r="A68" s="10" t="inlineStr">
-        <is>
-          <t>🏭 Ø Consumer Discretionary</t>
-        </is>
-      </c>
-      <c r="B68" s="11" t="inlineStr"/>
-      <c r="C68" s="12" t="inlineStr">
-        <is>
-          <t>Consumer Discretionary</t>
-        </is>
-      </c>
-      <c r="D68" s="13" t="inlineStr"/>
-      <c r="E68" s="13" t="inlineStr"/>
-      <c r="F68" s="14" t="inlineStr">
+      <c r="A68" s="11" t="inlineStr">
+        <is>
+          <t>🏭 Ø Real Estate</t>
+        </is>
+      </c>
+      <c r="B68" s="12" t="inlineStr"/>
+      <c r="C68" s="13" t="inlineStr">
+        <is>
+          <t>Real Estate</t>
+        </is>
+      </c>
+      <c r="D68" s="14" t="inlineStr"/>
+      <c r="E68" s="14" t="inlineStr"/>
+      <c r="F68" s="15" t="inlineStr">
         <is>
           <t>GICS-Sektor-Durchschnitt</t>
         </is>
       </c>
-      <c r="G68" s="14" t="inlineStr">
+      <c r="G68" s="15" t="inlineStr">
         <is>
           <t>GICS-Sektor-Ø (Refinitiv-Branchendurchschnitt)</t>
         </is>
       </c>
-      <c r="H68" s="12" t="inlineStr"/>
+      <c r="H68" s="13" t="inlineStr"/>
       <c r="I68" s="16" t="n">
-        <v>1174177883.9365</v>
+        <v>1089427082.8994</v>
       </c>
       <c r="J68" s="16" t="n">
-        <v>914241256.7812001</v>
+        <v>1079279417.5606</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
@@ -3652,49 +3693,49 @@
         </is>
       </c>
       <c r="H69" s="7" t="inlineStr"/>
-      <c r="I69" s="15" t="n">
-        <v>3546266335.8448</v>
-      </c>
-      <c r="J69" s="15" t="n">
-        <v>2918721581.658</v>
+      <c r="I69" s="10" t="n">
+        <v>3575065425.64</v>
+      </c>
+      <c r="J69" s="10" t="n">
+        <v>2937549836.9451</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="10" t="inlineStr">
-        <is>
-          <t>🏭 Ø Real Estate</t>
-        </is>
-      </c>
-      <c r="B70" s="11" t="inlineStr"/>
-      <c r="C70" s="12" t="inlineStr">
-        <is>
-          <t>Real Estate</t>
-        </is>
-      </c>
-      <c r="D70" s="13" t="inlineStr"/>
-      <c r="E70" s="13" t="inlineStr"/>
-      <c r="F70" s="14" t="inlineStr">
+      <c r="A70" s="11" t="inlineStr">
+        <is>
+          <t>🏭 Ø Consumer Discretionary</t>
+        </is>
+      </c>
+      <c r="B70" s="12" t="inlineStr"/>
+      <c r="C70" s="13" t="inlineStr">
+        <is>
+          <t>Consumer Discretionary</t>
+        </is>
+      </c>
+      <c r="D70" s="14" t="inlineStr"/>
+      <c r="E70" s="14" t="inlineStr"/>
+      <c r="F70" s="15" t="inlineStr">
         <is>
           <t>GICS-Sektor-Durchschnitt</t>
         </is>
       </c>
-      <c r="G70" s="14" t="inlineStr">
+      <c r="G70" s="15" t="inlineStr">
         <is>
           <t>GICS-Sektor-Ø (Refinitiv-Branchendurchschnitt)</t>
         </is>
       </c>
-      <c r="H70" s="12" t="inlineStr"/>
+      <c r="H70" s="13" t="inlineStr"/>
       <c r="I70" s="16" t="n">
-        <v>1090122599.1533</v>
+        <v>1179370856.2807</v>
       </c>
       <c r="J70" s="16" t="n">
-        <v>1080237304.3735</v>
+        <v>921661400.5118001</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="17" t="inlineStr">
-        <is>
-          <t>📅 Generated: 2025-08-29 15:23:29 | 📊 Companies: 57</t>
+      <c r="A71" s="18" t="inlineStr">
+        <is>
+          <t>📅 Generated: 2025-09-02 13:48:16 | 📊 Companies: 57</t>
         </is>
       </c>
     </row>

</xml_diff>